<commit_message>
Updated Stargen for Elevated Plains
* I just- had an idea for smth- have really high plains as well
</commit_message>
<xml_diff>
--- a/Stargen.xlsx
+++ b/Stargen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi\Documents\GitHub\Stargen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DCAF13-BD94-4116-A943-526F3CC7B8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133BB3FE-367F-402A-AA12-80E4801746B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t xml:space="preserve">        Aussie Mountain (Upscale)</t>
   </si>
@@ -129,13 +129,16 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">        Weblands</t>
-  </si>
-  <si>
-    <t>Flower Forest</t>
-  </si>
-  <si>
-    <t>hingeland but minecraft sussy</t>
+    <t xml:space="preserve">    Higher Plains</t>
+  </si>
+  <si>
+    <t>Taiga Mountains</t>
+  </si>
+  <si>
+    <t>Snowy Taiga</t>
+  </si>
+  <si>
+    <t>Snowy Tundra</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,11 +612,38 @@
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
         <v>35</v>
       </c>
-      <c r="C36" t="s">
-        <v>36</v>
+      <c r="C39" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GUYS I FIGURED OUT RIVERS
- Removed Pack.mcmeta
- Removed Pack.png
- Removed Surafac Folder
- Removed Noise Settings
- Removed Caves Folder
- Removed Cavefe Folder
+ Added HingeIsWet Surface Builder
+ Added Emriver Feature
+ Added Bamboo River test feature
+ Added Emriver to Taiga Mountains
+ Added Emriver to Taiga Hills
+ Added Bamboo River to Plains
+ Added Jungle as a waterfall test
  ^ Needs to be fixed and removed
+ Added Emriver to desert
</commit_message>
<xml_diff>
--- a/Stargen.xlsx
+++ b/Stargen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andi\Documents\GitHub\Stargen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879B2284-8F51-4343-9E0C-ED65E43FD524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9959BD-C698-45D9-A3A0-7855D32554EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t xml:space="preserve">        Aussie Mountain (Upscale)</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>coarse dirt instead of grass, lots of sand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Red Desert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Red Desert</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,7 @@
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="99" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -869,10 +875,16 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75">
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
       <c r="C52" s="2"/>
     </row>
     <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>63</v>
+      </c>
       <c r="C53" s="1"/>
     </row>
   </sheetData>

</xml_diff>